<commit_message>
More work on ACPerformanceManager and more tests on CS300.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/COSTS/Costs.xlsx
+++ b/JPADSandBox_v2/out/CS300/COSTS/Costs.xlsx
@@ -177,16 +177,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>5014.969391685628</v>
+        <v>6911.9002781658055</v>
       </c>
       <c r="C2" t="n">
-        <v>1578.2922316167383</v>
+        <v>1512.9537795510419</v>
       </c>
       <c r="D2" t="n">
-        <v>5.014969391685629</v>
+        <v>4.319937673853629</v>
       </c>
       <c r="E2" t="n">
-        <v>3.8576687628350994</v>
+        <v>3.323028979887408</v>
       </c>
     </row>
     <row r="3">
@@ -194,16 +194,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>4814.370616018203</v>
+        <v>6635.424267039174</v>
       </c>
       <c r="C3" t="n">
-        <v>1515.1605423520687</v>
+        <v>1452.4356283690004</v>
       </c>
       <c r="D3" t="n">
-        <v>4.814370616018204</v>
+        <v>4.147140166899485</v>
       </c>
       <c r="E3" t="n">
-        <v>3.7033620123216955</v>
+        <v>3.1901078206919116</v>
       </c>
     </row>
     <row r="4">
@@ -211,16 +211,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>371.7667968752254</v>
+        <v>512.3889750942196</v>
       </c>
       <c r="C4" t="n">
-        <v>117.00104260935197</v>
+        <v>112.15741044730504</v>
       </c>
       <c r="D4" t="n">
-        <v>0.37176679687522546</v>
+        <v>0.32024310943388734</v>
       </c>
       <c r="E4" t="n">
-        <v>0.28597445913478886</v>
+        <v>0.24634085341068257</v>
       </c>
     </row>
     <row r="5">
@@ -228,16 +228,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>10201.106804579056</v>
+        <v>14059.713520299201</v>
       </c>
       <c r="C5" t="n">
-        <v>3210.4538165781587</v>
+        <v>3077.5468183673474</v>
       </c>
       <c r="D5" t="n">
-        <v>10.201106804579059</v>
+        <v>8.787320950187004</v>
       </c>
       <c r="E5" t="n">
-        <v>7.847005234291584</v>
+        <v>6.759477653990002</v>
       </c>
     </row>
     <row r="6"/>
@@ -246,16 +246,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>4575.550572551343</v>
+        <v>6578.612337722757</v>
       </c>
       <c r="C7" t="n">
         <v>1440.0</v>
       </c>
       <c r="D7" t="n">
-        <v>4.575550572551344</v>
+        <v>4.111632711076724</v>
       </c>
       <c r="E7" t="n">
-        <v>3.5196542865779574</v>
+        <v>3.162794393135942</v>
       </c>
     </row>
     <row r="8">
@@ -263,16 +263,16 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>1143.8876431378358</v>
+        <v>1644.6530844306892</v>
       </c>
       <c r="C8" t="n">
         <v>360.0</v>
       </c>
       <c r="D8" t="n">
-        <v>1.143887643137836</v>
+        <v>1.027908177769181</v>
       </c>
       <c r="E8" t="n">
-        <v>0.8799135716444894</v>
+        <v>0.7906985982839855</v>
       </c>
     </row>
     <row r="9">
@@ -280,16 +280,16 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>5719.43821568918</v>
+        <v>8223.265422153447</v>
       </c>
       <c r="C9" t="n">
         <v>1800.0</v>
       </c>
       <c r="D9" t="n">
-        <v>5.719438215689181</v>
+        <v>5.1395408888459055</v>
       </c>
       <c r="E9" t="n">
-        <v>4.399567858222447</v>
+        <v>3.9534929914199273</v>
       </c>
     </row>
     <row r="10"/>
@@ -298,16 +298,16 @@
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>2363.806312414901</v>
+        <v>3824.4379904672924</v>
       </c>
       <c r="C11" t="n">
-        <v>743.9281974714229</v>
+        <v>837.1356182053528</v>
       </c>
       <c r="D11" t="n">
-        <v>2.363806312414902</v>
+        <v>2.3902737440420583</v>
       </c>
       <c r="E11" t="n">
-        <v>1.818312548011463</v>
+        <v>1.8386721108015833</v>
       </c>
     </row>
     <row r="12"/>
@@ -319,13 +319,13 @@
         <v>527.1629999999998</v>
       </c>
       <c r="C13" t="n">
-        <v>165.90674891758755</v>
+        <v>115.39131370412589</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5271629999999999</v>
+        <v>0.32947687499999995</v>
       </c>
       <c r="E13" t="n">
-        <v>0.40551</v>
+        <v>0.25344374999999997</v>
       </c>
     </row>
     <row r="14">
@@ -333,16 +333,16 @@
         <v>14</v>
       </c>
       <c r="B14" t="n">
-        <v>1076.591988266678</v>
+        <v>1722.5471812266846</v>
       </c>
       <c r="C14" t="n">
-        <v>338.82096559137534</v>
+        <v>377.0503281889781</v>
       </c>
       <c r="D14" t="n">
-        <v>1.0765919882666783</v>
+        <v>1.0765919882666781</v>
       </c>
       <c r="E14" t="n">
-        <v>0.8281476832820602</v>
+        <v>0.8281476832820601</v>
       </c>
     </row>
     <row r="15">
@@ -353,13 +353,13 @@
         <v>1325.9999999999995</v>
       </c>
       <c r="C15" t="n">
-        <v>417.3137133386089</v>
+        <v>290.24966086707707</v>
       </c>
       <c r="D15" t="n">
-        <v>1.3259999999999998</v>
+        <v>0.82875</v>
       </c>
       <c r="E15" t="n">
-        <v>1.02</v>
+        <v>0.6375</v>
       </c>
     </row>
     <row r="16">
@@ -370,13 +370,13 @@
         <v>5.446727122517808</v>
       </c>
       <c r="C16" t="n">
-        <v>1.7141733944494901</v>
+        <v>1.1922403470183296</v>
       </c>
       <c r="D16" t="n">
-        <v>0.005446727122517809</v>
+        <v>0.0034042044515736314</v>
       </c>
       <c r="E16" t="n">
-        <v>0.004189790094244469</v>
+        <v>0.0026186188089027933</v>
       </c>
     </row>
     <row r="17">
@@ -387,13 +387,13 @@
         <v>49.71055714285711</v>
       </c>
       <c r="C17" t="n">
-        <v>15.644718848730633</v>
+        <v>10.881200868950028</v>
       </c>
       <c r="D17" t="n">
-        <v>0.049710557142857124</v>
+        <v>0.031069098214285704</v>
       </c>
       <c r="E17" t="n">
-        <v>0.038238890109890095</v>
+        <v>0.023899306318681313</v>
       </c>
     </row>
     <row r="18">
@@ -401,16 +401,16 @@
         <v>18</v>
       </c>
       <c r="B18" t="n">
-        <v>2792.4977775320513</v>
+        <v>3438.4529704920587</v>
       </c>
       <c r="C18" t="n">
-        <v>878.8443567358321</v>
+        <v>752.6469144741434</v>
       </c>
       <c r="D18" t="n">
-        <v>2.792497777532052</v>
+        <v>2.149033106557537</v>
       </c>
       <c r="E18" t="n">
-        <v>2.148075213486194</v>
+        <v>1.653102389659644</v>
       </c>
     </row>
     <row r="19"/>
@@ -419,16 +419,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>1274.1492460300137</v>
+        <v>1645.838998047033</v>
       </c>
       <c r="C20" t="n">
-        <v>400.9954398253198</v>
+        <v>360.2595859916753</v>
       </c>
       <c r="D20" t="n">
-        <v>1.2741492460300141</v>
+        <v>1.028649373779396</v>
       </c>
       <c r="E20" t="n">
-        <v>0.9801148046384723</v>
+        <v>0.7912687490610738</v>
       </c>
     </row>
     <row r="21">
@@ -436,16 +436,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>4070.9335509099337</v>
+        <v>5583.811547390809</v>
       </c>
       <c r="C21" t="n">
-        <v>1281.188836263163</v>
+        <v>1222.246914008938</v>
       </c>
       <c r="D21" t="n">
-        <v>4.070933550909935</v>
+        <v>3.4898822171192565</v>
       </c>
       <c r="E21" t="n">
-        <v>3.131487346853796</v>
+        <v>2.684524782399428</v>
       </c>
     </row>
     <row r="22">
@@ -453,16 +453,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>5464.461070068991</v>
+        <v>7350.0095367655185</v>
       </c>
       <c r="C22" t="n">
-        <v>1719.75455546362</v>
+        <v>1608.8520176591062</v>
       </c>
       <c r="D22" t="n">
-        <v>5.464461070068992</v>
+        <v>4.59375596047845</v>
       </c>
       <c r="E22" t="n">
-        <v>4.203431592360763</v>
+        <v>3.5336584311372694</v>
       </c>
     </row>
     <row r="23"/>
@@ -472,16 +472,16 @@
         <v>22</v>
       </c>
       <c r="B25" t="n">
-        <v>26541.31018028418</v>
+        <v>36895.879440177516</v>
       </c>
       <c r="C25" t="n">
-        <v>8352.980926249034</v>
+        <v>8076.181368705949</v>
       </c>
       <c r="D25" t="n">
-        <v>26.54131018028419</v>
+        <v>23.059924650110954</v>
       </c>
       <c r="E25" t="n">
-        <v>20.416392446372456</v>
+        <v>17.738403577008423</v>
       </c>
     </row>
     <row r="26"/>
@@ -490,16 +490,16 @@
         <v>23</v>
       </c>
       <c r="B27" t="n">
-        <v>16340.203375705125</v>
+        <v>22836.165919878316</v>
       </c>
       <c r="C27" t="n">
-        <v>5142.527109670876</v>
+        <v>4998.634550338602</v>
       </c>
       <c r="D27" t="n">
-        <v>16.34020337570513</v>
+        <v>14.272603699923952</v>
       </c>
       <c r="E27" t="n">
-        <v>12.56938721208087</v>
+        <v>10.978925923018425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More tests on IRON canard and CS300.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/COSTS/Costs.xlsx
+++ b/JPADSandBox_v2/out/CS300/COSTS/Costs.xlsx
@@ -177,16 +177,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>6911.9002781658055</v>
+        <v>5043.814381988261</v>
       </c>
       <c r="C2" t="n">
-        <v>1512.9537795510419</v>
+        <v>1559.1962603120014</v>
       </c>
       <c r="D2" t="n">
-        <v>4.319937673853629</v>
+        <v>12.609535954970655</v>
       </c>
       <c r="E2" t="n">
-        <v>3.323028979887408</v>
+        <v>8.406357303313769</v>
       </c>
     </row>
     <row r="3">
@@ -194,16 +194,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>6635.424267039174</v>
+        <v>4842.061806708731</v>
       </c>
       <c r="C3" t="n">
-        <v>1452.4356283690004</v>
+        <v>1496.8284098995214</v>
       </c>
       <c r="D3" t="n">
-        <v>4.147140166899485</v>
+        <v>12.10515451677183</v>
       </c>
       <c r="E3" t="n">
-        <v>3.1901078206919116</v>
+        <v>8.07010301118122</v>
       </c>
     </row>
     <row r="4">
@@ -211,16 +211,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>512.3889750942196</v>
+        <v>371.1009409278338</v>
       </c>
       <c r="C4" t="n">
-        <v>112.15741044730504</v>
+        <v>114.71857516391253</v>
       </c>
       <c r="D4" t="n">
-        <v>0.32024310943388734</v>
+        <v>0.9277523523195847</v>
       </c>
       <c r="E4" t="n">
-        <v>0.24634085341068257</v>
+        <v>0.6185015682130565</v>
       </c>
     </row>
     <row r="5">
@@ -228,16 +228,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>14059.713520299201</v>
+        <v>10256.977129624825</v>
       </c>
       <c r="C5" t="n">
-        <v>3077.5468183673474</v>
+        <v>3170.7432453754354</v>
       </c>
       <c r="D5" t="n">
-        <v>8.787320950187004</v>
+        <v>25.64244282406207</v>
       </c>
       <c r="E5" t="n">
-        <v>6.759477653990002</v>
+        <v>17.094961882708045</v>
       </c>
     </row>
     <row r="6"/>
@@ -246,16 +246,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>6578.612337722757</v>
+        <v>4658.228662381298</v>
       </c>
       <c r="C7" t="n">
         <v>1440.0</v>
       </c>
       <c r="D7" t="n">
-        <v>4.111632711076724</v>
+        <v>11.645571655953248</v>
       </c>
       <c r="E7" t="n">
-        <v>3.162794393135942</v>
+        <v>7.7637144373021645</v>
       </c>
     </row>
     <row r="8">
@@ -263,16 +263,16 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>1644.6530844306892</v>
+        <v>873.4178741964934</v>
       </c>
       <c r="C8" t="n">
-        <v>360.0</v>
+        <v>270.0</v>
       </c>
       <c r="D8" t="n">
-        <v>1.027908177769181</v>
+        <v>2.183544685491234</v>
       </c>
       <c r="E8" t="n">
-        <v>0.7906985982839855</v>
+        <v>1.455696456994156</v>
       </c>
     </row>
     <row r="9">
@@ -280,16 +280,16 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>8223.265422153447</v>
+        <v>5531.646536577791</v>
       </c>
       <c r="C9" t="n">
-        <v>1800.0</v>
+        <v>1710.0</v>
       </c>
       <c r="D9" t="n">
-        <v>5.1395408888459055</v>
+        <v>13.829116341444482</v>
       </c>
       <c r="E9" t="n">
-        <v>3.9534929914199273</v>
+        <v>9.21941089429632</v>
       </c>
     </row>
     <row r="10"/>
@@ -298,16 +298,16 @@
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>3824.4379904672924</v>
+        <v>2024.9926550824753</v>
       </c>
       <c r="C11" t="n">
-        <v>837.1356182053528</v>
+        <v>625.9867504718206</v>
       </c>
       <c r="D11" t="n">
-        <v>2.3902737440420583</v>
+        <v>5.062481637706189</v>
       </c>
       <c r="E11" t="n">
-        <v>1.8386721108015833</v>
+        <v>3.374987758470793</v>
       </c>
     </row>
     <row r="12"/>
@@ -316,16 +316,16 @@
         <v>13</v>
       </c>
       <c r="B13" t="n">
-        <v>527.1629999999998</v>
+        <v>508.2557999999998</v>
       </c>
       <c r="C13" t="n">
-        <v>115.39131370412589</v>
+        <v>157.11730896994152</v>
       </c>
       <c r="D13" t="n">
-        <v>0.32947687499999995</v>
+        <v>1.2706395</v>
       </c>
       <c r="E13" t="n">
-        <v>0.25344374999999997</v>
+        <v>0.847093</v>
       </c>
     </row>
     <row r="14">
@@ -333,16 +333,16 @@
         <v>14</v>
       </c>
       <c r="B14" t="n">
-        <v>1722.5471812266846</v>
+        <v>422.84368226946447</v>
       </c>
       <c r="C14" t="n">
-        <v>377.0503281889781</v>
+        <v>130.71382849564975</v>
       </c>
       <c r="D14" t="n">
-        <v>1.0765919882666781</v>
+        <v>1.0571092056736615</v>
       </c>
       <c r="E14" t="n">
-        <v>0.8281476832820601</v>
+        <v>0.7047394704491077</v>
       </c>
     </row>
     <row r="15">
@@ -353,13 +353,13 @@
         <v>1325.9999999999995</v>
       </c>
       <c r="C15" t="n">
-        <v>290.24966086707707</v>
+        <v>409.9068848680968</v>
       </c>
       <c r="D15" t="n">
-        <v>0.82875</v>
+        <v>3.315</v>
       </c>
       <c r="E15" t="n">
-        <v>0.6375</v>
+        <v>2.21</v>
       </c>
     </row>
     <row r="16">
@@ -370,13 +370,13 @@
         <v>5.446727122517808</v>
       </c>
       <c r="C16" t="n">
-        <v>1.1922403470183296</v>
+        <v>1.6837488291989808</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0034042044515736314</v>
+        <v>0.013616817806294526</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0026186188089027933</v>
+        <v>0.009077878537529683</v>
       </c>
     </row>
     <row r="17">
@@ -387,13 +387,13 @@
         <v>49.71055714285711</v>
       </c>
       <c r="C17" t="n">
-        <v>10.881200868950028</v>
+        <v>15.367043456626009</v>
       </c>
       <c r="D17" t="n">
-        <v>0.031069098214285704</v>
+        <v>0.12427639285714281</v>
       </c>
       <c r="E17" t="n">
-        <v>0.023899306318681313</v>
+        <v>0.08285092857142855</v>
       </c>
     </row>
     <row r="18">
@@ -401,16 +401,16 @@
         <v>18</v>
       </c>
       <c r="B18" t="n">
-        <v>3438.4529704920587</v>
+        <v>2126.7433995348383</v>
       </c>
       <c r="C18" t="n">
-        <v>752.6469144741434</v>
+        <v>657.4409968454843</v>
       </c>
       <c r="D18" t="n">
-        <v>2.149033106557537</v>
+        <v>5.316858498837098</v>
       </c>
       <c r="E18" t="n">
-        <v>1.653102389659644</v>
+        <v>3.5445723325580656</v>
       </c>
     </row>
     <row r="19"/>
@@ -419,16 +419,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>1645.838998047033</v>
+        <v>1217.9944208403222</v>
       </c>
       <c r="C20" t="n">
-        <v>360.2595859916753</v>
+        <v>376.51907905986303</v>
       </c>
       <c r="D20" t="n">
-        <v>1.028649373779396</v>
+        <v>3.044986052100806</v>
       </c>
       <c r="E20" t="n">
-        <v>0.7912687490610738</v>
+        <v>2.0299907014005374</v>
       </c>
     </row>
     <row r="21">
@@ -436,16 +436,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>5583.811547390809</v>
+        <v>4391.925517902091</v>
       </c>
       <c r="C21" t="n">
-        <v>1222.246914008938</v>
+        <v>1357.6776075535065</v>
       </c>
       <c r="D21" t="n">
-        <v>3.4898822171192565</v>
+        <v>10.97981379475523</v>
       </c>
       <c r="E21" t="n">
-        <v>2.684524782399428</v>
+        <v>7.319875863170154</v>
       </c>
     </row>
     <row r="22">
@@ -453,16 +453,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>7350.0095367655185</v>
+        <v>5720.064789494046</v>
       </c>
       <c r="C22" t="n">
-        <v>1608.8520176591062</v>
+        <v>1768.2458062633418</v>
       </c>
       <c r="D22" t="n">
-        <v>4.59375596047845</v>
+        <v>14.300161973735118</v>
       </c>
       <c r="E22" t="n">
-        <v>3.5336584311372694</v>
+        <v>9.533441315823412</v>
       </c>
     </row>
     <row r="23"/>
@@ -472,16 +472,16 @@
         <v>22</v>
       </c>
       <c r="B25" t="n">
-        <v>36895.879440177516</v>
+        <v>25660.424510313973</v>
       </c>
       <c r="C25" t="n">
-        <v>8076.181368705949</v>
+        <v>7932.416798956081</v>
       </c>
       <c r="D25" t="n">
-        <v>23.059924650110954</v>
+        <v>64.15106127578495</v>
       </c>
       <c r="E25" t="n">
-        <v>17.738403577008423</v>
+        <v>42.76737418385663</v>
       </c>
     </row>
     <row r="26"/>
@@ -490,16 +490,16 @@
         <v>23</v>
       </c>
       <c r="B27" t="n">
-        <v>22836.165919878316</v>
+        <v>15403.447380689151</v>
       </c>
       <c r="C27" t="n">
-        <v>4998.634550338602</v>
+        <v>4761.673553580647</v>
       </c>
       <c r="D27" t="n">
-        <v>14.272603699923952</v>
+        <v>38.50861845172289</v>
       </c>
       <c r="E27" t="n">
-        <v>10.978925923018425</v>
+        <v>25.67241230114859</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More tests on CS300
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/COSTS/Costs.xlsx
+++ b/JPADSandBox_v2/out/CS300/COSTS/Costs.xlsx
@@ -177,16 +177,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>5043.814381988261</v>
+        <v>6999.995406508379</v>
       </c>
       <c r="C2" t="n">
-        <v>1559.1962603120014</v>
+        <v>1491.7477344706822</v>
       </c>
       <c r="D2" t="n">
-        <v>12.609535954970655</v>
+        <v>4.374997129067738</v>
       </c>
       <c r="E2" t="n">
-        <v>8.406357303313769</v>
+        <v>2.9166647527118257</v>
       </c>
     </row>
     <row r="3">
@@ -194,16 +194,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>4842.061806708731</v>
+        <v>6719.995590248043</v>
       </c>
       <c r="C3" t="n">
-        <v>1496.8284098995214</v>
+        <v>1432.0778250918547</v>
       </c>
       <c r="D3" t="n">
-        <v>12.10515451677183</v>
+        <v>4.199997243905028</v>
       </c>
       <c r="E3" t="n">
-        <v>8.07010301118122</v>
+        <v>2.7999981626033517</v>
       </c>
     </row>
     <row r="4">
@@ -211,16 +211,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>371.1009409278338</v>
+        <v>516.2783123628941</v>
       </c>
       <c r="C4" t="n">
-        <v>114.71857516391253</v>
+        <v>110.02250117301881</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9277523523195847</v>
+        <v>0.3226739452268089</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6185015682130565</v>
+        <v>0.21511596348453926</v>
       </c>
     </row>
     <row r="5">
@@ -228,16 +228,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>10256.977129624825</v>
+        <v>14236.269309119318</v>
       </c>
       <c r="C5" t="n">
-        <v>3170.7432453754354</v>
+        <v>3033.848060735556</v>
       </c>
       <c r="D5" t="n">
-        <v>25.64244282406207</v>
+        <v>8.897668318199576</v>
       </c>
       <c r="E5" t="n">
-        <v>17.094961882708045</v>
+        <v>5.931778878799717</v>
       </c>
     </row>
     <row r="6"/>
@@ -246,16 +246,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>4658.228662381298</v>
+        <v>6757.170232236857</v>
       </c>
       <c r="C7" t="n">
         <v>1440.0</v>
       </c>
       <c r="D7" t="n">
-        <v>11.645571655953248</v>
+        <v>4.223231395148037</v>
       </c>
       <c r="E7" t="n">
-        <v>7.7637144373021645</v>
+        <v>2.815487596765358</v>
       </c>
     </row>
     <row r="8">
@@ -263,16 +263,16 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>873.4178741964934</v>
+        <v>1266.969418544411</v>
       </c>
       <c r="C8" t="n">
         <v>270.0</v>
       </c>
       <c r="D8" t="n">
-        <v>2.183544685491234</v>
+        <v>0.7918558865902571</v>
       </c>
       <c r="E8" t="n">
-        <v>1.455696456994156</v>
+        <v>0.5279039243935046</v>
       </c>
     </row>
     <row r="9">
@@ -280,16 +280,16 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>5531.646536577791</v>
+        <v>8024.139650781269</v>
       </c>
       <c r="C9" t="n">
         <v>1710.0</v>
       </c>
       <c r="D9" t="n">
-        <v>13.829116341444482</v>
+        <v>5.015087281738294</v>
       </c>
       <c r="E9" t="n">
-        <v>9.21941089429632</v>
+        <v>3.3433915211588627</v>
       </c>
     </row>
     <row r="10"/>
@@ -298,16 +298,16 @@
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>2024.9926550824753</v>
+        <v>3452.2578682970907</v>
       </c>
       <c r="C11" t="n">
-        <v>625.9867504718206</v>
+        <v>735.7001761819095</v>
       </c>
       <c r="D11" t="n">
-        <v>5.062481637706189</v>
+        <v>2.1576611676856823</v>
       </c>
       <c r="E11" t="n">
-        <v>3.374987758470793</v>
+        <v>1.4384407784571216</v>
       </c>
     </row>
     <row r="12"/>
@@ -316,16 +316,16 @@
         <v>13</v>
       </c>
       <c r="B13" t="n">
-        <v>508.2557999999998</v>
+        <v>508.4273999999998</v>
       </c>
       <c r="C13" t="n">
-        <v>157.11730896994152</v>
+        <v>108.34941711356552</v>
       </c>
       <c r="D13" t="n">
-        <v>1.2706395</v>
+        <v>0.317767125</v>
       </c>
       <c r="E13" t="n">
-        <v>0.847093</v>
+        <v>0.21184475</v>
       </c>
     </row>
     <row r="14">
@@ -333,16 +333,16 @@
         <v>14</v>
       </c>
       <c r="B14" t="n">
-        <v>422.84368226946447</v>
+        <v>1691.6602304037292</v>
       </c>
       <c r="C14" t="n">
-        <v>130.71382849564975</v>
+        <v>360.50456745337505</v>
       </c>
       <c r="D14" t="n">
-        <v>1.0571092056736615</v>
+        <v>1.057287644002331</v>
       </c>
       <c r="E14" t="n">
-        <v>0.7047394704491077</v>
+        <v>0.7048584293348874</v>
       </c>
     </row>
     <row r="15">
@@ -353,13 +353,13 @@
         <v>1325.9999999999995</v>
       </c>
       <c r="C15" t="n">
-        <v>409.9068848680968</v>
+        <v>282.57982770517066</v>
       </c>
       <c r="D15" t="n">
-        <v>3.315</v>
+        <v>0.82875</v>
       </c>
       <c r="E15" t="n">
-        <v>2.21</v>
+        <v>0.5525</v>
       </c>
     </row>
     <row r="16">
@@ -370,13 +370,13 @@
         <v>5.446727122517808</v>
       </c>
       <c r="C16" t="n">
-        <v>1.6837488291989808</v>
+        <v>1.1607354538749344</v>
       </c>
       <c r="D16" t="n">
-        <v>0.013616817806294526</v>
+        <v>0.0034042044515736314</v>
       </c>
       <c r="E16" t="n">
-        <v>0.009077878537529683</v>
+        <v>0.002269469634382421</v>
       </c>
     </row>
     <row r="17">
@@ -387,13 +387,13 @@
         <v>49.71055714285711</v>
       </c>
       <c r="C17" t="n">
-        <v>15.367043456626009</v>
+        <v>10.593665665578136</v>
       </c>
       <c r="D17" t="n">
-        <v>0.12427639285714281</v>
+        <v>0.031069098214285704</v>
       </c>
       <c r="E17" t="n">
-        <v>0.08285092857142855</v>
+        <v>0.020712732142857137</v>
       </c>
     </row>
     <row r="18">
@@ -401,16 +401,16 @@
         <v>18</v>
       </c>
       <c r="B18" t="n">
-        <v>2126.7433995348383</v>
+        <v>3395.668913669103</v>
       </c>
       <c r="C18" t="n">
-        <v>657.4409968454843</v>
+        <v>723.6406761451127</v>
       </c>
       <c r="D18" t="n">
-        <v>5.316858498837098</v>
+        <v>2.12229307104319</v>
       </c>
       <c r="E18" t="n">
-        <v>3.5445723325580656</v>
+        <v>1.4148620473621265</v>
       </c>
     </row>
     <row r="19"/>
@@ -419,16 +419,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>1217.9944208403222</v>
+        <v>1609.158191191197</v>
       </c>
       <c r="C20" t="n">
-        <v>376.51907905986303</v>
+        <v>342.92280876106537</v>
       </c>
       <c r="D20" t="n">
-        <v>3.044986052100806</v>
+        <v>1.0057238694944983</v>
       </c>
       <c r="E20" t="n">
-        <v>2.0299907014005374</v>
+        <v>0.670482579662999</v>
       </c>
     </row>
     <row r="21">
@@ -436,16 +436,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>4391.925517902091</v>
+        <v>5937.368638487978</v>
       </c>
       <c r="C21" t="n">
-        <v>1357.6776075535065</v>
+        <v>1265.2945753288216</v>
       </c>
       <c r="D21" t="n">
-        <v>10.97981379475523</v>
+        <v>3.7108553990549877</v>
       </c>
       <c r="E21" t="n">
-        <v>7.319875863170154</v>
+        <v>2.473903599369992</v>
       </c>
     </row>
     <row r="22">
@@ -453,16 +453,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>5720.064789494046</v>
+        <v>7655.283504533765</v>
       </c>
       <c r="C22" t="n">
-        <v>1768.2458062633418</v>
+        <v>1631.3941883449377</v>
       </c>
       <c r="D22" t="n">
-        <v>14.300161973735118</v>
+        <v>4.784552190333605</v>
       </c>
       <c r="E22" t="n">
-        <v>9.533441315823412</v>
+        <v>3.1897014602224028</v>
       </c>
     </row>
     <row r="23"/>
@@ -472,16 +472,16 @@
         <v>22</v>
       </c>
       <c r="B25" t="n">
-        <v>25660.424510313973</v>
+        <v>36763.61924640054</v>
       </c>
       <c r="C25" t="n">
-        <v>7932.416798956081</v>
+        <v>7834.583101407516</v>
       </c>
       <c r="D25" t="n">
-        <v>64.15106127578495</v>
+        <v>22.977262029000347</v>
       </c>
       <c r="E25" t="n">
-        <v>42.76737418385663</v>
+        <v>15.318174686000232</v>
       </c>
     </row>
     <row r="26"/>
@@ -490,16 +490,16 @@
         <v>23</v>
       </c>
       <c r="B27" t="n">
-        <v>15403.447380689151</v>
+        <v>22527.34993728123</v>
       </c>
       <c r="C27" t="n">
-        <v>4761.673553580647</v>
+        <v>4800.735040671961</v>
       </c>
       <c r="D27" t="n">
-        <v>38.50861845172289</v>
+        <v>14.079593710800772</v>
       </c>
       <c r="E27" t="n">
-        <v>25.67241230114859</v>
+        <v>9.386395807200515</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More tests on IRON and CS300
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/COSTS/Costs.xlsx
+++ b/JPADSandBox_v2/out/CS300/COSTS/Costs.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Description</t>
   </si>
@@ -60,12 +60,6 @@
   </si>
   <si>
     <t>Ground handling charges</t>
-  </si>
-  <si>
-    <t>Noise charges</t>
-  </si>
-  <si>
-    <t>Emissions charges</t>
   </si>
   <si>
     <t>DOC Charges</t>
@@ -177,16 +171,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>6999.995406508379</v>
+        <v>3681.3780048128924</v>
       </c>
       <c r="C2" t="n">
-        <v>1491.7477344706822</v>
+        <v>1748.5715758377078</v>
       </c>
       <c r="D2" t="n">
-        <v>4.374997129067738</v>
+        <v>9.203445012032233</v>
       </c>
       <c r="E2" t="n">
-        <v>2.9166647527118257</v>
+        <v>7.079573086178641</v>
       </c>
     </row>
     <row r="3">
@@ -194,16 +188,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>6719.995590248043</v>
+        <v>3534.1228846203758</v>
       </c>
       <c r="C3" t="n">
-        <v>1432.0778250918547</v>
+        <v>1678.628712804199</v>
       </c>
       <c r="D3" t="n">
-        <v>4.199997243905028</v>
+        <v>8.835307211550942</v>
       </c>
       <c r="E3" t="n">
-        <v>2.7999981626033517</v>
+        <v>6.796390162731494</v>
       </c>
     </row>
     <row r="4">
@@ -211,16 +205,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>516.2783123628941</v>
+        <v>284.8530279732553</v>
       </c>
       <c r="C4" t="n">
-        <v>110.02250117301881</v>
+        <v>135.29876784023787</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3226739452268089</v>
+        <v>0.7121325699331384</v>
       </c>
       <c r="E4" t="n">
-        <v>0.21511596348453926</v>
+        <v>0.5477942845639525</v>
       </c>
     </row>
     <row r="5">
@@ -228,16 +222,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>14236.269309119318</v>
+        <v>7500.353917406524</v>
       </c>
       <c r="C5" t="n">
-        <v>3033.848060735556</v>
+        <v>3562.4990564821446</v>
       </c>
       <c r="D5" t="n">
-        <v>8.897668318199576</v>
+        <v>18.750884793516313</v>
       </c>
       <c r="E5" t="n">
-        <v>5.931778878799717</v>
+        <v>14.423757533474088</v>
       </c>
     </row>
     <row r="6"/>
@@ -246,16 +240,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>6757.170232236857</v>
+        <v>1515.861403726315</v>
       </c>
       <c r="C7" t="n">
-        <v>1440.0</v>
+        <v>720.0</v>
       </c>
       <c r="D7" t="n">
-        <v>4.223231395148037</v>
+        <v>3.7896535093157886</v>
       </c>
       <c r="E7" t="n">
-        <v>2.815487596765358</v>
+        <v>2.9151180840890683</v>
       </c>
     </row>
     <row r="8">
@@ -263,16 +257,16 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>1266.969418544411</v>
+        <v>568.4480263973682</v>
       </c>
       <c r="C8" t="n">
         <v>270.0</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7918558865902571</v>
+        <v>1.4211200659934209</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5279039243935046</v>
+        <v>1.0931692815334004</v>
       </c>
     </row>
     <row r="9">
@@ -280,16 +274,16 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>8024.139650781269</v>
+        <v>2084.3094301236833</v>
       </c>
       <c r="C9" t="n">
-        <v>1710.0</v>
+        <v>990.0</v>
       </c>
       <c r="D9" t="n">
-        <v>5.015087281738294</v>
+        <v>5.21077357530921</v>
       </c>
       <c r="E9" t="n">
-        <v>3.3433915211588627</v>
+        <v>4.0082873656224685</v>
       </c>
     </row>
     <row r="10"/>
@@ -298,16 +292,16 @@
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>3452.2578682970907</v>
+        <v>1176.1781334499897</v>
       </c>
       <c r="C11" t="n">
-        <v>735.7001761819095</v>
+        <v>558.6581029124803</v>
       </c>
       <c r="D11" t="n">
-        <v>2.1576611676856823</v>
+        <v>2.940445333624975</v>
       </c>
       <c r="E11" t="n">
-        <v>1.4384407784571216</v>
+        <v>2.2618810258653657</v>
       </c>
     </row>
     <row r="12"/>
@@ -319,13 +313,13 @@
         <v>508.4273999999998</v>
       </c>
       <c r="C13" t="n">
-        <v>108.34941711356552</v>
+        <v>241.4915552966295</v>
       </c>
       <c r="D13" t="n">
-        <v>0.317767125</v>
+        <v>1.2710685</v>
       </c>
       <c r="E13" t="n">
-        <v>0.21184475</v>
+        <v>0.977745</v>
       </c>
     </row>
     <row r="14">
@@ -333,16 +327,16 @@
         <v>14</v>
       </c>
       <c r="B14" t="n">
-        <v>1691.6602304037292</v>
+        <v>422.9150576009323</v>
       </c>
       <c r="C14" t="n">
-        <v>360.50456745337505</v>
+        <v>200.8751200631847</v>
       </c>
       <c r="D14" t="n">
         <v>1.057287644002331</v>
       </c>
       <c r="E14" t="n">
-        <v>0.7048584293348874</v>
+        <v>0.8132981876941008</v>
       </c>
     </row>
     <row r="15">
@@ -353,13 +347,13 @@
         <v>1325.9999999999995</v>
       </c>
       <c r="C15" t="n">
-        <v>282.57982770517066</v>
+        <v>629.8201126125987</v>
       </c>
       <c r="D15" t="n">
-        <v>0.82875</v>
+        <v>3.315</v>
       </c>
       <c r="E15" t="n">
-        <v>0.5525</v>
+        <v>2.55</v>
       </c>
     </row>
     <row r="16">
@@ -367,139 +361,105 @@
         <v>16</v>
       </c>
       <c r="B16" t="n">
-        <v>5.446727122517808</v>
+        <v>2257.342457600931</v>
       </c>
       <c r="C16" t="n">
-        <v>1.1607354538749344</v>
+        <v>1072.1867879724125</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0034042044515736314</v>
+        <v>5.643356144002329</v>
       </c>
       <c r="E16" t="n">
-        <v>0.002269469634382421</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="n">
-        <v>49.71055714285711</v>
-      </c>
-      <c r="C17" t="n">
-        <v>10.593665665578136</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.031069098214285704</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.020712732142857137</v>
-      </c>
-    </row>
+        <v>4.341043187694099</v>
+      </c>
+    </row>
+    <row r="17"/>
     <row r="18">
       <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1264.691245797864</v>
+      </c>
+      <c r="C18" t="n">
+        <v>600.6998362357305</v>
+      </c>
+      <c r="D18" t="n">
+        <v>3.161728114494661</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2.4320985496112777</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B18" t="n">
-        <v>3395.668913669103</v>
-      </c>
-      <c r="C18" t="n">
-        <v>723.6406761451127</v>
-      </c>
-      <c r="D18" t="n">
-        <v>2.12229307104319</v>
-      </c>
-      <c r="E18" t="n">
-        <v>1.4148620473621265</v>
-      </c>
-    </row>
-    <row r="19"/>
+      <c r="B19" t="n">
+        <v>1739.3323710475756</v>
+      </c>
+      <c r="C19" t="n">
+        <v>826.1436725519779</v>
+      </c>
+      <c r="D19" t="n">
+        <v>4.348330927618941</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3.3448699443222623</v>
+      </c>
+    </row>
     <row r="20">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>1609.158191191197</v>
+        <v>3115.8838918840343</v>
       </c>
       <c r="C20" t="n">
-        <v>342.92280876106537</v>
+        <v>1479.9746181554942</v>
       </c>
       <c r="D20" t="n">
-        <v>1.0057238694944983</v>
+        <v>7.789709729710088</v>
       </c>
       <c r="E20" t="n">
-        <v>0.670482579662999</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
+        <v>5.9920844074692985</v>
+      </c>
+    </row>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23">
+      <c r="A23" t="s">
         <v>20</v>
       </c>
-      <c r="B21" t="n">
-        <v>5937.368638487978</v>
-      </c>
-      <c r="C21" t="n">
-        <v>1265.2945753288216</v>
-      </c>
-      <c r="D21" t="n">
-        <v>3.7108553990549877</v>
-      </c>
-      <c r="E21" t="n">
-        <v>2.473903599369992</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" t="n">
-        <v>7655.283504533765</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1631.3941883449377</v>
-      </c>
-      <c r="D22" t="n">
-        <v>4.784552190333605</v>
-      </c>
-      <c r="E22" t="n">
-        <v>3.1897014602224028</v>
-      </c>
-    </row>
-    <row r="23"/>
+      <c r="B23" t="n">
+        <v>16134.067830465163</v>
+      </c>
+      <c r="C23" t="n">
+        <v>7663.3185655225325</v>
+      </c>
+      <c r="D23" t="n">
+        <v>40.33516957616292</v>
+      </c>
+      <c r="E23" t="n">
+        <v>31.027053520125325</v>
+      </c>
+    </row>
     <row r="24"/>
     <row r="25">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" t="n">
-        <v>36763.61924640054</v>
+        <v>8633.713913058638</v>
       </c>
       <c r="C25" t="n">
-        <v>7834.583101407516</v>
+        <v>4100.819509040387</v>
       </c>
       <c r="D25" t="n">
-        <v>22.977262029000347</v>
+        <v>21.584284782646602</v>
       </c>
       <c r="E25" t="n">
-        <v>15.318174686000232</v>
-      </c>
-    </row>
-    <row r="26"/>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" t="n">
-        <v>22527.34993728123</v>
-      </c>
-      <c r="C27" t="n">
-        <v>4800.735040671961</v>
-      </c>
-      <c r="D27" t="n">
-        <v>14.079593710800772</v>
-      </c>
-      <c r="E27" t="n">
-        <v>9.386395807200515</v>
+        <v>16.603295986651233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More work on ACPerformanceManager: Mission profile
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/COSTS/Costs.xlsx
+++ b/JPADSandBox_v2/out/CS300/COSTS/Costs.xlsx
@@ -171,16 +171,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>3681.335999999998</v>
+        <v>2684.6999999999985</v>
       </c>
       <c r="C2" t="n">
-        <v>1748.5763141228617</v>
+        <v>1917.6428571428569</v>
       </c>
       <c r="D2" t="n">
-        <v>9.203339999999995</v>
+        <v>6.711749999999996</v>
       </c>
       <c r="E2" t="n">
-        <v>7.079492307692304</v>
+        <v>5.162884615384613</v>
       </c>
     </row>
     <row r="3">
@@ -188,16 +188,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>3534.082559999998</v>
+        <v>2577.3119999999985</v>
       </c>
       <c r="C3" t="n">
-        <v>1678.6332615579472</v>
+        <v>1840.9371428571426</v>
       </c>
       <c r="D3" t="n">
-        <v>8.835206399999995</v>
+        <v>6.443279999999996</v>
       </c>
       <c r="E3" t="n">
-        <v>6.796312615384611</v>
+        <v>4.956369230769228</v>
       </c>
     </row>
     <row r="4">
@@ -205,16 +205,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>284.8497777777778</v>
+        <v>207.7333333333333</v>
       </c>
       <c r="C4" t="n">
-        <v>135.29913447329534</v>
+        <v>148.3809523809524</v>
       </c>
       <c r="D4" t="n">
-        <v>0.7121244444444444</v>
+        <v>0.5193333333333332</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5477880341880342</v>
+        <v>0.39948717948717943</v>
       </c>
     </row>
     <row r="5">
@@ -222,16 +222,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>7500.268337777773</v>
+        <v>5469.74533333333</v>
       </c>
       <c r="C5" t="n">
-        <v>3562.508710154104</v>
+        <v>3906.9609523809513</v>
       </c>
       <c r="D5" t="n">
-        <v>18.750670844444432</v>
+        <v>13.674363333333325</v>
       </c>
       <c r="E5" t="n">
-        <v>14.42359295726495</v>
+        <v>10.518741025641019</v>
       </c>
     </row>
     <row r="6"/>
@@ -240,16 +240,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>1515.84</v>
+        <v>1007.9999999999997</v>
       </c>
       <c r="C7" t="n">
         <v>720.0</v>
       </c>
       <c r="D7" t="n">
-        <v>3.7895999999999996</v>
+        <v>2.519999999999999</v>
       </c>
       <c r="E7" t="n">
-        <v>2.915076923076923</v>
+        <v>1.9384615384615378</v>
       </c>
     </row>
     <row r="8">
@@ -257,16 +257,16 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>568.4399999999999</v>
+        <v>377.99999999999983</v>
       </c>
       <c r="C8" t="n">
         <v>270.0</v>
       </c>
       <c r="D8" t="n">
-        <v>1.4210999999999998</v>
+        <v>0.9449999999999996</v>
       </c>
       <c r="E8" t="n">
-        <v>1.0931538461538461</v>
+        <v>0.7269230769230766</v>
       </c>
     </row>
     <row r="9">
@@ -274,16 +274,16 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>2084.2799999999997</v>
+        <v>1385.9999999999995</v>
       </c>
       <c r="C9" t="n">
         <v>990.0</v>
       </c>
       <c r="D9" t="n">
-        <v>5.210699999999999</v>
+        <v>3.464999999999999</v>
       </c>
       <c r="E9" t="n">
-        <v>4.00823076923077</v>
+        <v>2.665384615384614</v>
       </c>
     </row>
     <row r="10"/>
@@ -292,16 +292,16 @@
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>1313.497927396606</v>
+        <v>672.9592695723795</v>
       </c>
       <c r="C11" t="n">
-        <v>623.8907191560827</v>
+        <v>480.68519255169986</v>
       </c>
       <c r="D11" t="n">
-        <v>3.283744818491515</v>
+        <v>1.6823981739309488</v>
       </c>
       <c r="E11" t="n">
-        <v>2.5259575526857807</v>
+        <v>1.2941524414853451</v>
       </c>
     </row>
     <row r="12"/>
@@ -313,7 +313,7 @@
         <v>508.4273999999998</v>
       </c>
       <c r="C13" t="n">
-        <v>241.49496516782764</v>
+        <v>363.16242857142856</v>
       </c>
       <c r="D13" t="n">
         <v>1.2710684999999995</v>
@@ -330,7 +330,7 @@
         <v>422.9150576009323</v>
       </c>
       <c r="C14" t="n">
-        <v>200.8779564285619</v>
+        <v>302.082184000666</v>
       </c>
       <c r="D14" t="n">
         <v>1.0572876440023307</v>
@@ -347,7 +347,7 @@
         <v>1325.9999999999995</v>
       </c>
       <c r="C15" t="n">
-        <v>629.8290056998098</v>
+        <v>947.1428571428572</v>
       </c>
       <c r="D15" t="n">
         <v>3.314999999999999</v>
@@ -364,7 +364,7 @@
         <v>2257.342457600931</v>
       </c>
       <c r="C16" t="n">
-        <v>1072.201927296199</v>
+        <v>1612.3874697149513</v>
       </c>
       <c r="D16" t="n">
         <v>5.643356144002328</v>
@@ -379,16 +379,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>1264.6811855601686</v>
+        <v>1025.9848466230153</v>
       </c>
       <c r="C18" t="n">
-        <v>600.7035396897571</v>
+        <v>732.8463190164398</v>
       </c>
       <c r="D18" t="n">
-        <v>3.1617029639004217</v>
+        <v>2.5649621165575383</v>
       </c>
       <c r="E18" t="n">
-        <v>2.4320792030003244</v>
+        <v>1.973047781967337</v>
       </c>
     </row>
     <row r="19">
@@ -396,16 +396,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>1739.3130881928244</v>
+        <v>1281.7943920165299</v>
       </c>
       <c r="C19" t="n">
-        <v>826.1461786856354</v>
+        <v>915.5674228689502</v>
       </c>
       <c r="D19" t="n">
-        <v>4.348282720482061</v>
+        <v>3.2044859800413246</v>
       </c>
       <c r="E19" t="n">
-        <v>3.3448328619092775</v>
+        <v>2.4649892154164035</v>
       </c>
     </row>
     <row r="20">
@@ -413,16 +413,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>3115.854584453671</v>
+        <v>2420.485693246031</v>
       </c>
       <c r="C20" t="n">
-        <v>1479.9815948956639</v>
+        <v>1728.9183523185943</v>
       </c>
       <c r="D20" t="n">
-        <v>7.789636461134178</v>
+        <v>6.051214233115077</v>
       </c>
       <c r="E20" t="n">
-        <v>5.992028047026291</v>
+        <v>4.654780179319291</v>
       </c>
     </row>
     <row r="21"/>
@@ -432,16 +432,16 @@
         <v>20</v>
       </c>
       <c r="B23" t="n">
-        <v>16271.24330722898</v>
+        <v>12206.532753752672</v>
       </c>
       <c r="C23" t="n">
-        <v>7728.58295150205</v>
+        <v>8718.951966966197</v>
       </c>
       <c r="D23" t="n">
-        <v>40.67810826807245</v>
+        <v>30.516331884381678</v>
       </c>
       <c r="E23" t="n">
-        <v>31.290852513901886</v>
+        <v>23.47410144952437</v>
       </c>
     </row>
     <row r="24"/>
@@ -450,16 +450,16 @@
         <v>21</v>
       </c>
       <c r="B25" t="n">
-        <v>8770.974969451208</v>
+        <v>6736.787420419341</v>
       </c>
       <c r="C25" t="n">
-        <v>4166.074241347946</v>
+        <v>4811.9910145852455</v>
       </c>
       <c r="D25" t="n">
-        <v>21.92743742362802</v>
+        <v>16.841968551048353</v>
       </c>
       <c r="E25" t="n">
-        <v>16.867259556636938</v>
+        <v>12.955360423883349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>